<commit_message>
added Factor and Quality Req doc
</commit_message>
<xml_diff>
--- a/Timechart.xlsx
+++ b/Timechart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="17">
   <si>
     <t>Nils</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Assignment planning</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Factors and Issues</t>
   </si>
 </sst>
 </file>
@@ -108,10 +114,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G31"/>
+  <dimension ref="A2:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,20 +424,29 @@
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -446,8 +462,23 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -455,8 +486,15 @@
         <f>SUM(B6:F6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <f>SUM(J6:N6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -467,8 +505,16 @@
         <f>SUM(B7:F7)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="O7">
+        <f>SUM(J7:N7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -476,8 +522,15 @@
         <f>SUM(B8:F8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>SUM(J8:N8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -485,19 +538,33 @@
         <f>SUM(B9:F9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <f>SUM(J9:N9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="G10" s="1">
         <f>SUM(G6:G9)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="O10" s="1">
+        <f>SUM(O6:O9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="K11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -513,8 +580,23 @@
       <c r="F12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="J12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -522,8 +604,15 @@
         <f>SUM(B13:F13)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f>SUM(J13:N13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -531,8 +620,15 @@
         <f>SUM(B14:F14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <f>SUM(J14:N14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -540,8 +636,15 @@
         <f>SUM(B15:F15)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="I15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>SUM(J15:N15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -549,19 +652,33 @@
         <f>SUM(B16:F16)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16">
+        <f>SUM(J16:N16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="G17" s="1">
         <f>SUM(G13:G16)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="O17" s="1">
+        <f>SUM(O13:O16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="C18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -577,8 +694,23 @@
       <c r="F19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="J19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -586,8 +718,15 @@
         <f>SUM(B20:F20)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="I20" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <f>SUM(J20:N20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -595,8 +734,15 @@
         <f>SUM(B21:F21)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="I21" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <f>SUM(J21:N21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -604,8 +750,15 @@
         <f>SUM(B22:F22)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="I22" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>SUM(J22:N22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -613,19 +766,33 @@
         <f>SUM(B23:F23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="I23" t="s">
+        <v>3</v>
+      </c>
+      <c r="O23">
+        <f>SUM(J23:N23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="G24" s="1">
         <f>SUM(G20:G23)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="O24" s="1">
+        <f>SUM(O20:O23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="C25" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -641,8 +808,23 @@
       <c r="F26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="J26" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" t="s">
+        <v>5</v>
+      </c>
+      <c r="L26" t="s">
+        <v>6</v>
+      </c>
+      <c r="M26" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -653,8 +835,16 @@
         <f>SUM(B27:F27)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="I27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="O27">
+        <f>SUM(J27:N27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -665,8 +855,16 @@
         <f>SUM(B28:F28)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="I28" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="O28">
+        <f>SUM(J28:N28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -677,8 +875,16 @@
         <f>SUM(B29:F29)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="I29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="O29">
+        <f>SUM(J29:N29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -689,11 +895,164 @@
         <f>SUM(B30:F30)</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="O30">
+        <f>SUM(J30:N30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="G31" s="1">
         <f>SUM(G27:G30)</f>
         <v>5</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="O31" s="1">
+        <f>SUM(O27:O30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" t="s">
+        <v>5</v>
+      </c>
+      <c r="L35" t="s">
+        <v>6</v>
+      </c>
+      <c r="M35" t="s">
+        <v>7</v>
+      </c>
+      <c r="N35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="G36">
+        <f>SUM(B36:F36)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" s="3"/>
+      <c r="K36" s="2">
+        <v>4</v>
+      </c>
+      <c r="O36">
+        <f>SUM(J36:N36)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="G37">
+        <f>SUM(B37:F37)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="K37" s="2">
+        <v>4</v>
+      </c>
+      <c r="O37">
+        <f>SUM(J37:N37)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="G38">
+        <f>SUM(B38:F38)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3"/>
+      <c r="K38" s="2">
+        <v>4</v>
+      </c>
+      <c r="O38">
+        <f>SUM(J38:N38)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="G39">
+        <f>SUM(B39:F39)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>3</v>
+      </c>
+      <c r="J39" s="3"/>
+      <c r="K39" s="2">
+        <v>4</v>
+      </c>
+      <c r="O39">
+        <f>SUM(J39:N39)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="B40" s="3"/>
+      <c r="G40" s="1">
+        <f>SUM(G36:G39)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="3"/>
+      <c r="O40" s="1">
+        <f>SUM(O36:O39)</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last update from school
</commit_message>
<xml_diff>
--- a/Timechart.xlsx
+++ b/Timechart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="19">
   <si>
     <t>Nils</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Factors and Issues</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Total hours</t>
   </si>
 </sst>
 </file>
@@ -114,11 +120,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,18 +427,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O40"/>
+  <dimension ref="A2:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4:W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" customWidth="1"/>
+    <col min="25" max="27" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -445,15 +455,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="K4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -484,8 +497,23 @@
       <c r="N5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" t="s">
+        <v>7</v>
+      </c>
+      <c r="V5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -500,8 +528,18 @@
         <f>SUM(J6:N6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <f>SUM(R6:V6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -520,8 +558,18 @@
         <f>SUM(J7:N7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q7" t="s">
+        <v>2</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <f>SUM(R7:V7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -536,8 +584,18 @@
         <f>SUM(J8:N8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="W8">
+        <f>SUM(R8:V8)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -552,8 +610,18 @@
         <f>SUM(J9:N9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q9" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="W9">
+        <f>SUM(R9:V9)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G10" s="1">
         <f>SUM(G6:G9)</f>
         <v>0.5</v>
@@ -562,8 +630,12 @@
         <f>SUM(O6:O9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W10" s="1">
+        <f>SUM(W6:W9)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>10</v>
       </c>
@@ -571,7 +643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -602,8 +674,11 @@
       <c r="N12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -618,8 +693,23 @@
         <f>SUM(J13:N13)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" t="s">
+        <v>5</v>
+      </c>
+      <c r="T13" t="s">
+        <v>6</v>
+      </c>
+      <c r="U13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -634,8 +724,18 @@
         <f>SUM(J14:N14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" s="2">
+        <v>3</v>
+      </c>
+      <c r="W14">
+        <f>SUM(R14:V14)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -650,8 +750,18 @@
         <f>SUM(J15:N15)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q15" t="s">
+        <v>2</v>
+      </c>
+      <c r="U15" s="2">
+        <v>3</v>
+      </c>
+      <c r="W15">
+        <f>SUM(R15:V15)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -666,8 +776,15 @@
         <f>SUM(J16:N16)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <f>SUM(R16:V16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G17" s="1">
         <f>SUM(G13:G16)</f>
         <v>0</v>
@@ -676,16 +793,30 @@
         <f>SUM(O13:O16)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>3</v>
+      </c>
+      <c r="U17" s="2">
+        <v>3</v>
+      </c>
+      <c r="W17">
+        <f>SUM(R17:V17)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>13</v>
       </c>
       <c r="K18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W18" s="1">
+        <f>SUM(W14:W17)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -717,7 +848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -729,14 +860,17 @@
         <v>1</v>
       </c>
       <c r="M20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O20">
         <f>SUM(J20:N20)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="S20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -748,14 +882,29 @@
         <v>2</v>
       </c>
       <c r="M21" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O21">
         <f>SUM(J21:N21)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="R21" t="s">
+        <v>4</v>
+      </c>
+      <c r="S21" t="s">
+        <v>5</v>
+      </c>
+      <c r="T21" t="s">
+        <v>6</v>
+      </c>
+      <c r="U21" t="s">
+        <v>7</v>
+      </c>
+      <c r="V21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -770,8 +919,25 @@
         <f>SUM(J22:N22)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3"/>
+      <c r="S22" s="2">
+        <v>4</v>
+      </c>
+      <c r="T22" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="U22" s="2">
+        <v>2</v>
+      </c>
+      <c r="W22">
+        <f>SUM(R22:V22)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -783,32 +949,77 @@
         <v>3</v>
       </c>
       <c r="M23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O23">
         <f>SUM(J23:N23)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>2</v>
+      </c>
+      <c r="R23" s="3"/>
+      <c r="S23" s="2">
+        <v>4</v>
+      </c>
+      <c r="T23" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="U23" s="2">
+        <v>2</v>
+      </c>
+      <c r="W23">
+        <f>SUM(R23:V23)</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G24" s="1">
         <f>SUM(G20:G23)</f>
         <v>0</v>
       </c>
       <c r="O24" s="1">
         <f>SUM(O20:O23)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" s="3"/>
+      <c r="S24" s="2">
+        <v>4</v>
+      </c>
+      <c r="T24" s="2">
+        <v>2</v>
+      </c>
+      <c r="W24">
+        <f>SUM(R24:V24)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="K25" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>3</v>
+      </c>
+      <c r="R25" s="3"/>
+      <c r="S25" s="2">
+        <v>4</v>
+      </c>
+      <c r="T25" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="W25">
+        <f>SUM(R25:V25)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -839,8 +1050,13 @@
       <c r="N26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R26" s="3"/>
+      <c r="W26" s="1">
+        <f>SUM(W22:W25)</f>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -860,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -879,8 +1095,14 @@
         <f>SUM(J28:N28)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R28" t="s">
+        <v>18</v>
+      </c>
+      <c r="S28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -899,8 +1121,19 @@
         <f>SUM(J29:N29)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <f>W6+W14+W22</f>
+        <v>11.5</v>
+      </c>
+      <c r="S29" s="4">
+        <f>R29/R33*100</f>
+        <v>26.436781609195403</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -919,8 +1152,19 @@
         <f>SUM(J30:N30)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>2</v>
+      </c>
+      <c r="R30">
+        <f>W7+W15+W23</f>
+        <v>12.5</v>
+      </c>
+      <c r="S30" s="4">
+        <f>R30/R33*100</f>
+        <v>28.735632183908045</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G31" s="1">
         <f>SUM(G27:G30)</f>
         <v>5</v>
@@ -930,8 +1174,42 @@
         <f>SUM(O27:O30)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f>W8+W16+W24</f>
+        <v>7.5</v>
+      </c>
+      <c r="S31" s="4">
+        <f>R31/R33*100</f>
+        <v>17.241379310344829</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R32">
+        <f>W9+W17+W25</f>
+        <v>12</v>
+      </c>
+      <c r="S32" s="4">
+        <f>R32/R33*100</f>
+        <v>27.586206896551722</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <f>W10+W18+W26</f>
+        <v>43.5</v>
+      </c>
+      <c r="S33">
+        <f>SUM(S29:S32)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>16</v>
       </c>
@@ -939,7 +1217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -971,7 +1249,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -999,7 +1277,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1027,7 +1305,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1077,7 +1355,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="G40" s="1">
         <f>SUM(G36:G39)</f>

</xml_diff>

<commit_message>
lots of changes everywhere
</commit_message>
<xml_diff>
--- a/Timechart.xlsx
+++ b/Timechart.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19155" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="A01" sheetId="1" r:id="rId1"/>
+    <sheet name="GA02" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="25">
   <si>
     <t>Nils</t>
   </si>
@@ -73,13 +73,31 @@
   </si>
   <si>
     <t>Total hours</t>
+  </si>
+  <si>
+    <t>Updating A01</t>
+  </si>
+  <si>
+    <t>Peer-evaluation</t>
+  </si>
+  <si>
+    <t>Modular view</t>
+  </si>
+  <si>
+    <t>Execution view</t>
+  </si>
+  <si>
+    <t>GA02</t>
+  </si>
+  <si>
+    <t>Architecture evaluation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,7 +233,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -250,7 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,14 +442,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4:W33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O40" sqref="A2:O40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -441,7 +457,7 @@
     <col min="25" max="27" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -455,7 +471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23">
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -466,7 +482,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -513,7 +529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -539,7 +555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -569,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -595,7 +611,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -621,7 +637,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23">
       <c r="G10" s="1">
         <f>SUM(G6:G9)</f>
         <v>0.5</v>
@@ -635,7 +651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23">
       <c r="C11" t="s">
         <v>10</v>
       </c>
@@ -643,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -678,7 +694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -709,7 +725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -735,7 +751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -761,7 +777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -784,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23">
       <c r="G17" s="1">
         <f>SUM(G13:G16)</f>
         <v>0</v>
@@ -804,7 +820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23">
       <c r="C18" t="s">
         <v>13</v>
       </c>
@@ -816,7 +832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -848,7 +864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -870,7 +886,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -904,7 +920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -937,7 +953,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -973,7 +989,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23">
       <c r="G24" s="1">
         <f>SUM(G20:G23)</f>
         <v>0</v>
@@ -997,7 +1013,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23">
       <c r="C25" t="s">
         <v>14</v>
       </c>
@@ -1019,7 +1035,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1072,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1076,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1102,7 +1118,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1149,7 @@
         <v>26.436781609195403</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +1180,7 @@
         <v>28.735632183908045</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23">
       <c r="G31" s="1">
         <f>SUM(G27:G30)</f>
         <v>5</v>
@@ -1186,7 +1202,7 @@
         <v>17.241379310344829</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23">
       <c r="Q32" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1215,7 @@
         <v>27.586206896551722</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="R33">
         <f>W10+W18+W26</f>
         <v>43.5</v>
@@ -1209,7 +1225,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="C34" t="s">
         <v>16</v>
       </c>
@@ -1217,7 +1233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="B35" t="s">
         <v>4</v>
       </c>
@@ -1249,7 +1265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1277,7 +1293,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1305,7 +1321,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1355,7 +1371,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19">
       <c r="B40" s="3"/>
       <c r="G40" s="1">
         <f>SUM(G36:G39)</f>
@@ -1374,24 +1390,934 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f>SUM(B5:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <f>SUM(J5:N5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="G6">
+        <f>SUM(B6:F6)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="O6">
+        <f>SUM(J6:N6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>SUM(B7:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>SUM(J7:N7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <f>SUM(B8:F8)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <f>SUM(J8:N8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="G9" s="1">
+        <f>SUM(G5:G8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <f>SUM(O5:O8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f>SUM(B12:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <f>SUM(J12:N12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <f>SUM(B13:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <f>SUM(J13:N13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>SUM(B14:F14)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>SUM(J14:N14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <f>SUM(B15:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15">
+        <f>SUM(J15:N15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="G16" s="1">
+        <f>SUM(G12:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <f>SUM(O12:O15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" t="s">
+        <v>5</v>
+      </c>
+      <c r="L18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f>SUM(B19:F19)</f>
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2">
+        <v>4</v>
+      </c>
+      <c r="O19">
+        <f>SUM(J19:N19)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f>SUM(B20:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <f>SUM(J20:N20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>SUM(B21:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>SUM(J21:N21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <f>SUM(B22:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="2">
+        <v>4</v>
+      </c>
+      <c r="O22">
+        <f>SUM(J22:N22)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="G23" s="1">
+        <f>SUM(G19:G22)</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <f>SUM(O19:O22)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" t="s">
+        <v>5</v>
+      </c>
+      <c r="L25" t="s">
+        <v>6</v>
+      </c>
+      <c r="M25" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>SUM(B26:F26)</f>
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="O26">
+        <f>SUM(J26:N26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f>SUM(B27:F27)</f>
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="O27">
+        <f>SUM(J27:N27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f>SUM(B28:F28)</f>
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="O28">
+        <f>SUM(J28:N28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f>SUM(B29:F29)</f>
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="O29">
+        <f>SUM(J29:N29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="G30" s="1">
+        <f>SUM(G26:G29)</f>
+        <v>4</v>
+      </c>
+      <c r="O30" s="1">
+        <f>SUM(O26:O29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" t="s">
+        <v>6</v>
+      </c>
+      <c r="M34" t="s">
+        <v>7</v>
+      </c>
+      <c r="N34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="2">
+        <v>3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <f>SUM(B35:F35)</f>
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="O35">
+        <f>SUM(J35:N35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="2">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <f>SUM(B36:F36)</f>
+        <v>5</v>
+      </c>
+      <c r="I36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="O36">
+        <f>SUM(J36:N36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <f>SUM(B37:F37)</f>
+        <v>3</v>
+      </c>
+      <c r="I37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="O37">
+        <f>SUM(J37:N37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="2">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <f>SUM(B38:F38)</f>
+        <v>5</v>
+      </c>
+      <c r="I38" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="O38">
+        <f>SUM(J38:N38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="B39" s="3"/>
+      <c r="G39" s="1">
+        <f>SUM(G35:G38)</f>
+        <v>18</v>
+      </c>
+      <c r="J39" s="3"/>
+      <c r="O39" s="1">
+        <f>SUM(O35:O38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+      <c r="J43" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" t="s">
+        <v>5</v>
+      </c>
+      <c r="L43" t="s">
+        <v>6</v>
+      </c>
+      <c r="M43" t="s">
+        <v>7</v>
+      </c>
+      <c r="N43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="G44">
+        <f>SUM(B44:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="O44">
+        <f>SUM(J44:N44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="G45">
+        <f>SUM(B45:F45)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="O45">
+        <f>SUM(J45:N45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="G46">
+        <f>SUM(B46:F46)</f>
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="O46">
+        <f>SUM(J46:N46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="G47">
+        <f>SUM(B47:F47)</f>
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>3</v>
+      </c>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="O47">
+        <f>SUM(J47:N47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="B48" s="3"/>
+      <c r="G48" s="1">
+        <f>SUM(G44:G47)</f>
+        <v>0</v>
+      </c>
+      <c r="J48" s="3"/>
+      <c r="O48" s="1">
+        <f>SUM(O44:O47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+      <c r="K51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" t="s">
+        <v>4</v>
+      </c>
+      <c r="K52" t="s">
+        <v>5</v>
+      </c>
+      <c r="L52" t="s">
+        <v>6</v>
+      </c>
+      <c r="M52" t="s">
+        <v>7</v>
+      </c>
+      <c r="N52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="G53">
+        <f>SUM(B53:F53)</f>
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>1</v>
+      </c>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="O53">
+        <f>SUM(J53:N53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="G54">
+        <f>SUM(B54:F54)</f>
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>2</v>
+      </c>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="O54">
+        <f>SUM(J54:N54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="G55">
+        <f>SUM(B55:F55)</f>
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="O55">
+        <f>SUM(J55:N55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="G56">
+        <f>SUM(B56:F56)</f>
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>3</v>
+      </c>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="O56">
+        <f>SUM(J56:N56)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="B57" s="3"/>
+      <c r="G57" s="1">
+        <f>SUM(G53:G56)</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="3"/>
+      <c r="O57" s="1">
+        <f>SUM(O53:O56)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>